<commit_message>
new look today; need to add hand search items
</commit_message>
<xml_diff>
--- a/Search_Results.xlsx
+++ b/Search_Results.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15160" windowHeight="17600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -410,7 +410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -648,7 +648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>

</xml_diff>